<commit_message>
excel doc has been updated
</commit_message>
<xml_diff>
--- a/Automated Alert Full Cloud Version/fire extinguisher data excel f.xlsx
+++ b/Automated Alert Full Cloud Version/fire extinguisher data excel f.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Automated-Alert\Automated Alert Full Cloud Version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F987CDF-9C06-4C32-8FA9-AECBF7FDA4FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0B7A29-0308-4FAF-A286-C04D8A47890A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{2B3651D7-ACB5-4F22-B3CD-6238BCB3B001}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,7 +634,7 @@
         <v>45776</v>
       </c>
       <c r="D9" s="3">
-        <v>45834</v>
+        <v>45835</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -648,7 +648,7 @@
         <v>45778</v>
       </c>
       <c r="D10" s="3">
-        <v>45818</v>
+        <v>45835</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>